<commit_message>
Added 10x versions 2 & 3 to assay_type in HCA scrnaseq (#674)
* Added 10x versions 2 & 3 to assay_type

Added these assay_types : scRNAseq-10xGenomics-v2, scRNAseq-10xGenomics-v3

* regen, changelog

Co-authored-by: mccalluc <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>donor_id</t>
   </si>
@@ -596,7 +596,10 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>scRNAseq-10xGenomics</t>
+    <t>scRNAseq-10xGenomics-v2</t>
+  </si>
+  <si>
+    <t>scRNAseq-10xGenomics-v3</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1097,97 +1100,97 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1195,8 +1198,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="I2:I1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: scRNAseq-10xGenomics / scRNAseq / sciRNAseq / snRNAseq / SNARE2-RNAseq." sqref="J2:J1048576">
-      <formula1>'assay_type list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="J2:J1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="K2:K1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1248,7 +1251,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1277,6 +1280,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1302,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mccalluc/add source for hca (#673)
* Add source_project

* regen

* changelog

* Lookup for source_project works now

* factor out _get_schema_version_from_row

* Add doctest

* move get_schema_version_from_row

* Fix tests

* doctest

* Add a new fixture

* Fix schemaloader doc tests

* Shorter error message

* Add -v3 to assay name

* better description, regen
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -8,10 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
-    <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
-    <sheet name="analyte_class list" sheetId="4" r:id="rId4"/>
-    <sheet name="library_final_yield_unit list" sheetId="5" r:id="rId5"/>
+    <sheet name="source_project list" sheetId="2" r:id="rId2"/>
+    <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
+    <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
+    <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
+    <sheet name="library_final_yield_unit list" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -32,11 +33,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>External source (outside of HuBMAP) of the project, eg. HCA (The Human Cell Atlas Consortium).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -283,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -348,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -387,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -439,7 +453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -452,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -465,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -478,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -517,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -543,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +575,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+  <si>
+    <t>source_project</t>
+  </si>
+  <si>
+    <t>HCA</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -1059,7 +1079,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1068,160 +1088,166 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="I2:I1048576">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: HCA." sqref="A2:A1048576">
+      <formula1>'source_project list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="J2:J1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="K2:K1048576">
       <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="L2:L1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="M2:M1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="AA2:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="AB2:AB1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AG2:AG1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AH2:AH1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AI2:AI1048576">
       <formula1>'library_final_yield_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AL2:AL1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AM2:AM1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AM2:AM1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1241,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1250,6 +1276,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -1259,49 +1303,31 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1320,7 +1346,25 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
factor out sc_isolation_entity (#825)
* factor out sc_isolation_entity

* Apply suggestions from code review

Co-authored-by: chris briggs <cebriggs7135@gmail.com>

* regen

Co-authored-by: chris briggs <cebriggs7135@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -12,7 +12,8 @@
     <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
     <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
-    <sheet name="library_final_yield_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="sc_isolation_entity list" sheetId="6" r:id="rId6"/>
+    <sheet name="library_final_yield_unit list" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -280,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A quality metric by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level.</t>
+          <t>A quality metric by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level. "OK" or "not OK", or with more specificity such as "debris", "clump", "low clump".</t>
         </r>
       </text>
     </comment>
@@ -575,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>source_project</t>
   </si>
@@ -653,6 +654,18 @@
   </si>
   <si>
     <t>sc_isolation_entity</t>
+  </si>
+  <si>
+    <t>whole cell</t>
+  </si>
+  <si>
+    <t>nucleus</t>
+  </si>
+  <si>
+    <t>cell-cell multimer</t>
+  </si>
+  <si>
+    <t>spatially encoded cell barcoding</t>
   </si>
   <si>
     <t>sc_isolation_tissue_dissociation</t>
@@ -1141,83 +1154,83 @@
         <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: HCA." sqref="A2:A1048576">
       <formula1>'source_project list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1232,6 +1245,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="M2:M1048576">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: whole cell / nucleus / cell-cell multimer / spatially encoded cell barcoding." sqref="Q2:Q1048576">
+      <formula1>'sc_isolation_entity list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="AB2:AB1048576">
       <formula1>"TRUE,FALSE"</formula1>
@@ -1356,6 +1372,39 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1364,7 +1413,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mccalluc/even more numeric fields (#1014)
* make integer

* regen
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -1217,7 +1217,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="14">
+  <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: HCA." sqref="A2:A1048576">
       <formula1>'source_project list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1234,6 +1234,10 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="V2:V1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add snRNAseq-10xGenomics-v2 to the scrnaseq assays
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>source_project</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>scRNAseq-10xGenomics-v3</t>
+  </si>
+  <si>
+    <t>snRNAseq-10xGenomics-v2</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1123,97 +1126,97 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1228,7 @@
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="K2:K1048576">
-      <formula1>'assay_type list'!$A$1:$A$6</formula1>
+      <formula1>'assay_type list'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="L2:L1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1315,7 +1318,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,6 +1352,11 @@
     <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1392,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Add snRNAseq-10xGenomics-v2 to the scrnaseq assays"
This reverts commit 94a3311a6eafab0870ad10b5b5a9fa462499848e.
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>source_project</t>
   </si>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>scRNAseq-10xGenomics-v3</t>
-  </si>
-  <si>
-    <t>snRNAseq-10xGenomics-v2</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1126,97 +1123,97 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="AJ1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1228,7 +1225,7 @@
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="K2:K1048576">
-      <formula1>'assay_type list'!$A$1:$A$7</formula1>
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="L2:L1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1318,7 +1315,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1352,11 +1349,6 @@
     <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1384,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add snRNAseq_10xGenomics_v2 to scrnaseq assay schemas
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>source_project</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>scRNAseq-10xGenomics-v3</t>
+  </si>
+  <si>
+    <t>snRNAseq-10xGenomics-v2</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1123,97 +1126,97 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1228,7 @@
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="K2:K1048576">
-      <formula1>'assay_type list'!$A$1:$A$6</formula1>
+      <formula1>'assay_type list'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="L2:L1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1315,7 +1318,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,6 +1352,11 @@
     <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1392,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add snRNAseq_10xGenomics_v2 to scrnaseq assay schemas (#1041)
</commit_message>
<xml_diff>
--- a/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
+++ b/docs/scrnaseq-hca/scrnaseq-hca-metadata.xlsx
@@ -575,7 +575,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>source_project</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>scRNAseq-10xGenomics-v3</t>
+  </si>
+  <si>
+    <t>snRNAseq-10xGenomics-v2</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1123,97 +1126,97 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1228,7 @@
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="K2:K1048576">
-      <formula1>'assay_type list'!$A$1:$A$6</formula1>
+      <formula1>'assay_type list'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="L2:L1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1315,7 +1318,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1349,6 +1352,11 @@
     <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1392,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>